<commit_message>
Add TestDVP_upgrade.ts to Unittests_DvP_SC.xlsx
</commit_message>
<xml_diff>
--- a/docs/Unittests_DvP_SC.xlsx
+++ b/docs/Unittests_DvP_SC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Projects\DLT2Pay\CMTA\Git\DvP_Contract\src\solidity\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Projects\DLT2Pay\CMTA\GitHubIntelliJ_Fork\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
   <si>
     <t>Test</t>
   </si>
@@ -207,6 +207,18 @@
   </si>
   <si>
     <t>implicitly covered by checkDelivery</t>
+  </si>
+  <si>
+    <t>Upgradeability</t>
+  </si>
+  <si>
+    <t>Tests that DvP can be upgraded and downgraded</t>
+  </si>
+  <si>
+    <t>TestDVP_upgrade.ts</t>
+  </si>
+  <si>
+    <t>"Tests DVP Upgradeability."</t>
   </si>
 </sst>
 </file>
@@ -271,8 +283,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:D29" totalsRowShown="0">
-  <autoFilter ref="A1:D29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:D30" totalsRowShown="0">
+  <autoFilter ref="A1:D30"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Function"/>
     <tableColumn id="2" name="Test"/>
@@ -546,9 +558,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -955,6 +969,20 @@
         <v>33</v>
       </c>
     </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -965,15 +993,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100CE8C848401DDED4CA9C0FC4CC73A1749" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="531d7f6ac7d45f6bd0366a6d8f6f15ed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="089b61df-ae7b-4f9a-b579-034449ba6e6e" xmlns:ns3="332f4895-888a-49a5-82d0-2478c4fd9930" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5ce8392a84116976b7d263c63598e79a" ns2:_="" ns3:_="">
     <xsd:import namespace="089b61df-ae7b-4f9a-b579-034449ba6e6e"/>
@@ -1190,6 +1209,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1197,14 +1225,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F639738F-E2E0-487F-A5D6-6A368ACC48F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB665D90-FEC8-449A-900E-F4717C92A219}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1219,6 +1239,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F639738F-E2E0-487F-A5D6-6A368ACC48F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>